<commit_message>
added cost as image
</commit_message>
<xml_diff>
--- a/Floodrisk.xlsx
+++ b/Floodrisk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viktoriapues/Documents/casa/Remote sensing/senseitmapitsorted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85E780C-BBC8-4B40-8193-5B54D42210B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7FCDDF-ACBC-0447-98EE-B4EA572A34B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="759" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -303,7 +303,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -446,8 +446,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF58595B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +546,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -638,7 +667,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -685,7 +714,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -758,6 +786,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="22" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,7 +1112,7 @@
   <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="118" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE34" sqref="AE34"/>
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1115,224 +1148,224 @@
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>0</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>1</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <v>2</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="29">
         <v>3</v>
       </c>
-      <c r="G4" s="30">
+      <c r="G4" s="29">
         <v>4</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="29">
         <v>5</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="29">
         <v>6</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="29">
         <v>7</v>
       </c>
-      <c r="K4" s="30">
+      <c r="K4" s="29">
         <v>8</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="29">
         <v>9</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="29">
         <v>10</v>
       </c>
-      <c r="N4" s="30">
+      <c r="N4" s="29">
         <v>11</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="29">
         <v>12</v>
       </c>
-      <c r="P4" s="30">
+      <c r="P4" s="29">
         <v>13</v>
       </c>
-      <c r="Q4" s="30">
+      <c r="Q4" s="29">
         <v>14</v>
       </c>
-      <c r="R4" s="30">
+      <c r="R4" s="29">
         <v>15</v>
       </c>
-      <c r="S4" s="30">
+      <c r="S4" s="29">
         <v>16</v>
       </c>
-      <c r="T4" s="30">
+      <c r="T4" s="29">
         <v>17</v>
       </c>
-      <c r="U4" s="30">
+      <c r="U4" s="29">
         <v>18</v>
       </c>
-      <c r="V4" s="30">
+      <c r="V4" s="29">
         <v>19</v>
       </c>
-      <c r="W4" s="30">
+      <c r="W4" s="29">
         <v>20</v>
       </c>
-      <c r="X4" s="30">
+      <c r="X4" s="29">
         <v>21</v>
       </c>
-      <c r="Y4" s="30">
+      <c r="Y4" s="29">
         <v>22</v>
       </c>
-      <c r="Z4" s="30">
+      <c r="Z4" s="29">
         <v>23</v>
       </c>
-      <c r="AA4" s="30">
+      <c r="AA4" s="29">
         <v>24</v>
       </c>
-      <c r="AB4" s="30">
+      <c r="AB4" s="29">
         <v>25</v>
       </c>
-      <c r="AC4" s="30">
+      <c r="AC4" s="29">
         <v>26</v>
       </c>
-      <c r="AD4" s="30">
+      <c r="AD4" s="29">
         <v>27</v>
       </c>
-      <c r="AE4" s="30">
+      <c r="AE4" s="29">
         <v>28</v>
       </c>
-      <c r="AF4" s="30">
+      <c r="AF4" s="29">
         <v>29</v>
       </c>
-      <c r="AG4" s="30">
+      <c r="AG4" s="29">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:33" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>45413</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="30">
         <f t="shared" ref="D5:AG5" si="0">C5+7</f>
         <v>45420</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <f t="shared" si="0"/>
         <v>45427</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <f t="shared" si="0"/>
         <v>45434</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="30">
         <f t="shared" si="0"/>
         <v>45441</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="30">
         <f t="shared" si="0"/>
         <v>45448</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="30">
         <f t="shared" si="0"/>
         <v>45455</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="30">
         <f t="shared" si="0"/>
         <v>45462</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="30">
         <f t="shared" si="0"/>
         <v>45469</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="30">
         <f t="shared" si="0"/>
         <v>45476</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="30">
         <f t="shared" si="0"/>
         <v>45483</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="30">
         <f t="shared" si="0"/>
         <v>45490</v>
       </c>
-      <c r="O5" s="31">
+      <c r="O5" s="30">
         <f t="shared" si="0"/>
         <v>45497</v>
       </c>
-      <c r="P5" s="31">
+      <c r="P5" s="30">
         <f t="shared" si="0"/>
         <v>45504</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="30">
         <f t="shared" si="0"/>
         <v>45511</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="30">
         <f t="shared" si="0"/>
         <v>45518</v>
       </c>
-      <c r="S5" s="31">
+      <c r="S5" s="30">
         <f t="shared" si="0"/>
         <v>45525</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="30">
         <f t="shared" si="0"/>
         <v>45532</v>
       </c>
-      <c r="U5" s="31">
+      <c r="U5" s="30">
         <f t="shared" si="0"/>
         <v>45539</v>
       </c>
-      <c r="V5" s="31">
+      <c r="V5" s="30">
         <f t="shared" si="0"/>
         <v>45546</v>
       </c>
-      <c r="W5" s="31">
+      <c r="W5" s="30">
         <f t="shared" si="0"/>
         <v>45553</v>
       </c>
-      <c r="X5" s="31">
+      <c r="X5" s="30">
         <f t="shared" si="0"/>
         <v>45560</v>
       </c>
-      <c r="Y5" s="31">
+      <c r="Y5" s="30">
         <f t="shared" si="0"/>
         <v>45567</v>
       </c>
-      <c r="Z5" s="31">
+      <c r="Z5" s="30">
         <f t="shared" si="0"/>
         <v>45574</v>
       </c>
-      <c r="AA5" s="31">
+      <c r="AA5" s="30">
         <f t="shared" si="0"/>
         <v>45581</v>
       </c>
-      <c r="AB5" s="31">
+      <c r="AB5" s="30">
         <f t="shared" si="0"/>
         <v>45588</v>
       </c>
-      <c r="AC5" s="31">
+      <c r="AC5" s="30">
         <f t="shared" si="0"/>
         <v>45595</v>
       </c>
-      <c r="AD5" s="31">
+      <c r="AD5" s="30">
         <f t="shared" si="0"/>
         <v>45602</v>
       </c>
-      <c r="AE5" s="31">
+      <c r="AE5" s="30">
         <f t="shared" si="0"/>
         <v>45609</v>
       </c>
-      <c r="AF5" s="31">
+      <c r="AF5" s="30">
         <f t="shared" si="0"/>
         <v>45616</v>
       </c>
-      <c r="AG5" s="31">
+      <c r="AG5" s="30">
         <f t="shared" si="0"/>
         <v>45623</v>
       </c>
@@ -1342,650 +1375,650 @@
       <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
-      <c r="AA6" s="32"/>
-      <c r="AB6" s="32"/>
-      <c r="AC6" s="32"/>
-      <c r="AD6" s="32"/>
-      <c r="AE6" s="32"/>
-      <c r="AF6" s="32"/>
-      <c r="AG6" s="32"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
+      <c r="Z6" s="31"/>
+      <c r="AA6" s="31"/>
+      <c r="AB6" s="31"/>
+      <c r="AC6" s="31"/>
+      <c r="AD6" s="31"/>
+      <c r="AE6" s="31"/>
+      <c r="AF6" s="31"/>
+      <c r="AG6" s="31"/>
     </row>
     <row r="7" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="36"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="36"/>
-      <c r="U7" s="36"/>
-      <c r="V7" s="36"/>
-      <c r="W7" s="36"/>
-      <c r="X7" s="36"/>
-      <c r="Y7" s="36"/>
-      <c r="Z7" s="36"/>
-      <c r="AA7" s="36"/>
-      <c r="AB7" s="36"/>
-      <c r="AC7" s="36"/>
-      <c r="AD7" s="36"/>
-      <c r="AE7" s="36"/>
-      <c r="AF7" s="36"/>
-      <c r="AG7" s="36"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35"/>
+      <c r="T7" s="35"/>
+      <c r="U7" s="35"/>
+      <c r="V7" s="35"/>
+      <c r="W7" s="35"/>
+      <c r="X7" s="35"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="35"/>
+      <c r="AB7" s="35"/>
+      <c r="AC7" s="35"/>
+      <c r="AD7" s="35"/>
+      <c r="AE7" s="35"/>
+      <c r="AF7" s="35"/>
+      <c r="AG7" s="35"/>
     </row>
     <row r="8" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="36"/>
-      <c r="U8" s="36"/>
-      <c r="V8" s="36"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="36"/>
-      <c r="Y8" s="36"/>
-      <c r="Z8" s="36"/>
-      <c r="AA8" s="36"/>
-      <c r="AB8" s="36"/>
-      <c r="AC8" s="36"/>
-      <c r="AD8" s="36"/>
-      <c r="AE8" s="36"/>
-      <c r="AF8" s="36"/>
-      <c r="AG8" s="36"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="35"/>
+      <c r="T8" s="35"/>
+      <c r="U8" s="35"/>
+      <c r="V8" s="35"/>
+      <c r="W8" s="35"/>
+      <c r="X8" s="35"/>
+      <c r="Y8" s="35"/>
+      <c r="Z8" s="35"/>
+      <c r="AA8" s="35"/>
+      <c r="AB8" s="35"/>
+      <c r="AC8" s="35"/>
+      <c r="AD8" s="35"/>
+      <c r="AE8" s="35"/>
+      <c r="AF8" s="35"/>
+      <c r="AG8" s="35"/>
     </row>
     <row r="9" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35" t="s">
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="M9" s="34"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="35" t="s">
+      <c r="M9" s="33"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="35" t="s">
+      <c r="Q9" s="35"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="U9" s="36"/>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="35" t="s">
+      <c r="U9" s="35"/>
+      <c r="V9" s="35"/>
+      <c r="W9" s="35"/>
+      <c r="X9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="Y9" s="36"/>
-      <c r="Z9" s="36"/>
-      <c r="AA9" s="36"/>
-      <c r="AB9" s="35" t="s">
+      <c r="Y9" s="35"/>
+      <c r="Z9" s="35"/>
+      <c r="AA9" s="35"/>
+      <c r="AB9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AC9" s="36"/>
-      <c r="AD9" s="36"/>
-      <c r="AE9" s="36"/>
-      <c r="AF9" s="35" t="s">
+      <c r="AC9" s="35"/>
+      <c r="AD9" s="35"/>
+      <c r="AE9" s="35"/>
+      <c r="AF9" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AG9" s="36"/>
+      <c r="AG9" s="35"/>
     </row>
     <row r="10" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="35" t="s">
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="36"/>
-      <c r="M10" s="35" t="s">
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="N10" s="37"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="35" t="s">
+      <c r="N10" s="36"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="R10" s="34"/>
-      <c r="S10" s="36"/>
-      <c r="T10" s="36"/>
-      <c r="U10" s="35" t="s">
+      <c r="R10" s="33"/>
+      <c r="S10" s="35"/>
+      <c r="T10" s="35"/>
+      <c r="U10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="V10" s="36"/>
-      <c r="W10" s="36"/>
-      <c r="X10" s="36"/>
-      <c r="Y10" s="35" t="s">
+      <c r="V10" s="35"/>
+      <c r="W10" s="35"/>
+      <c r="X10" s="35"/>
+      <c r="Y10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="Z10" s="36"/>
-      <c r="AA10" s="36"/>
-      <c r="AB10" s="36"/>
-      <c r="AC10" s="35" t="s">
+      <c r="Z10" s="35"/>
+      <c r="AA10" s="35"/>
+      <c r="AB10" s="35"/>
+      <c r="AC10" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AD10" s="36"/>
-      <c r="AE10" s="36"/>
-      <c r="AF10" s="36"/>
-      <c r="AG10" s="35" t="s">
+      <c r="AD10" s="35"/>
+      <c r="AE10" s="35"/>
+      <c r="AF10" s="35"/>
+      <c r="AG10" s="34" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="36"/>
-      <c r="S11" s="36"/>
-      <c r="T11" s="36"/>
-      <c r="U11" s="36"/>
-      <c r="V11" s="36"/>
-      <c r="W11" s="36"/>
-      <c r="X11" s="36"/>
-      <c r="Y11" s="36"/>
-      <c r="Z11" s="36"/>
-      <c r="AA11" s="36"/>
-      <c r="AB11" s="36"/>
-      <c r="AC11" s="36"/>
-      <c r="AD11" s="36"/>
-      <c r="AE11" s="36"/>
-      <c r="AF11" s="36"/>
-      <c r="AG11" s="36"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="35"/>
+      <c r="S11" s="35"/>
+      <c r="T11" s="35"/>
+      <c r="U11" s="35"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="35"/>
+      <c r="X11" s="35"/>
+      <c r="Y11" s="35"/>
+      <c r="Z11" s="35"/>
+      <c r="AA11" s="35"/>
+      <c r="AB11" s="35"/>
+      <c r="AC11" s="35"/>
+      <c r="AD11" s="35"/>
+      <c r="AE11" s="35"/>
+      <c r="AF11" s="35"/>
+      <c r="AG11" s="35"/>
     </row>
     <row r="12" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="36"/>
-      <c r="W12" s="36"/>
-      <c r="X12" s="36"/>
-      <c r="Y12" s="36"/>
-      <c r="Z12" s="36"/>
-      <c r="AA12" s="36"/>
-      <c r="AB12" s="36"/>
-      <c r="AC12" s="36"/>
-      <c r="AD12" s="36"/>
-      <c r="AE12" s="36"/>
-      <c r="AF12" s="36"/>
-      <c r="AG12" s="36"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="35"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="35"/>
+      <c r="V12" s="35"/>
+      <c r="W12" s="35"/>
+      <c r="X12" s="35"/>
+      <c r="Y12" s="35"/>
+      <c r="Z12" s="35"/>
+      <c r="AA12" s="35"/>
+      <c r="AB12" s="35"/>
+      <c r="AC12" s="35"/>
+      <c r="AD12" s="35"/>
+      <c r="AE12" s="35"/>
+      <c r="AF12" s="35"/>
+      <c r="AG12" s="35"/>
     </row>
     <row r="13" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="39" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="36"/>
-      <c r="T13" s="36"/>
-      <c r="U13" s="36"/>
-      <c r="V13" s="36"/>
-      <c r="W13" s="36"/>
-      <c r="X13" s="36"/>
-      <c r="Y13" s="36"/>
-      <c r="Z13" s="36"/>
-      <c r="AA13" s="36"/>
-      <c r="AB13" s="36"/>
-      <c r="AC13" s="36"/>
-      <c r="AD13" s="36"/>
-      <c r="AE13" s="36"/>
-      <c r="AF13" s="36"/>
-      <c r="AG13" s="36"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="35"/>
+      <c r="W13" s="35"/>
+      <c r="X13" s="35"/>
+      <c r="Y13" s="35"/>
+      <c r="Z13" s="35"/>
+      <c r="AA13" s="35"/>
+      <c r="AB13" s="35"/>
+      <c r="AC13" s="35"/>
+      <c r="AD13" s="35"/>
+      <c r="AE13" s="35"/>
+      <c r="AF13" s="35"/>
+      <c r="AG13" s="35"/>
     </row>
     <row r="14" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>1.2</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="36"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="36"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="36"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="36"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="36"/>
-      <c r="AA14" s="36"/>
-      <c r="AB14" s="36"/>
-      <c r="AC14" s="36"/>
-      <c r="AD14" s="36"/>
-      <c r="AE14" s="36"/>
-      <c r="AF14" s="36"/>
-      <c r="AG14" s="36"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="35"/>
+      <c r="Q14" s="35"/>
+      <c r="R14" s="35"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="35"/>
+      <c r="U14" s="35"/>
+      <c r="V14" s="35"/>
+      <c r="W14" s="35"/>
+      <c r="X14" s="35"/>
+      <c r="Y14" s="35"/>
+      <c r="Z14" s="35"/>
+      <c r="AA14" s="35"/>
+      <c r="AB14" s="35"/>
+      <c r="AC14" s="35"/>
+      <c r="AD14" s="35"/>
+      <c r="AE14" s="35"/>
+      <c r="AF14" s="35"/>
+      <c r="AG14" s="35"/>
     </row>
     <row r="15" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>1.2</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="40" t="s">
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="44" t="s">
+      <c r="I15" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="40" t="s">
+      <c r="J15" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="36"/>
-      <c r="Z15" s="36"/>
-      <c r="AA15" s="36"/>
-      <c r="AB15" s="36"/>
-      <c r="AC15" s="36"/>
-      <c r="AD15" s="36"/>
-      <c r="AE15" s="36"/>
-      <c r="AF15" s="36"/>
-      <c r="AG15" s="36"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="35"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="35"/>
+      <c r="R15" s="35"/>
+      <c r="S15" s="35"/>
+      <c r="T15" s="35"/>
+      <c r="U15" s="35"/>
+      <c r="V15" s="35"/>
+      <c r="W15" s="35"/>
+      <c r="X15" s="35"/>
+      <c r="Y15" s="35"/>
+      <c r="Z15" s="35"/>
+      <c r="AA15" s="35"/>
+      <c r="AB15" s="35"/>
+      <c r="AC15" s="35"/>
+      <c r="AD15" s="35"/>
+      <c r="AE15" s="35"/>
+      <c r="AF15" s="35"/>
+      <c r="AG15" s="35"/>
     </row>
     <row r="16" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
       <c r="B16" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="36"/>
-      <c r="AA16" s="36"/>
-      <c r="AB16" s="36"/>
-      <c r="AC16" s="36"/>
-      <c r="AD16" s="36"/>
-      <c r="AE16" s="36"/>
-      <c r="AF16" s="36"/>
-      <c r="AG16" s="36"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="44"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="44"/>
+      <c r="X16" s="44"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="35"/>
+      <c r="AA16" s="35"/>
+      <c r="AB16" s="35"/>
+      <c r="AC16" s="35"/>
+      <c r="AD16" s="35"/>
+      <c r="AE16" s="35"/>
+      <c r="AF16" s="35"/>
+      <c r="AG16" s="35"/>
     </row>
     <row r="17" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>2.1</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="46"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="46"/>
-      <c r="R17" s="36"/>
-      <c r="S17" s="36"/>
-      <c r="T17" s="36"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="36"/>
-      <c r="W17" s="36"/>
-      <c r="X17" s="36"/>
-      <c r="Y17" s="36"/>
-      <c r="Z17" s="36"/>
-      <c r="AA17" s="36"/>
-      <c r="AB17" s="36"/>
-      <c r="AC17" s="36"/>
-      <c r="AD17" s="36"/>
-      <c r="AE17" s="36"/>
-      <c r="AF17" s="36"/>
-      <c r="AG17" s="36"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="35"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
+      <c r="V17" s="35"/>
+      <c r="W17" s="35"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="35"/>
+      <c r="Z17" s="35"/>
+      <c r="AA17" s="35"/>
+      <c r="AB17" s="35"/>
+      <c r="AC17" s="35"/>
+      <c r="AD17" s="35"/>
+      <c r="AE17" s="35"/>
+      <c r="AF17" s="35"/>
+      <c r="AG17" s="35"/>
     </row>
     <row r="18" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="46"/>
-      <c r="R18" s="46"/>
-      <c r="S18" s="46"/>
-      <c r="T18" s="46"/>
-      <c r="U18" s="46"/>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="36"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="36"/>
-      <c r="AA18" s="36"/>
-      <c r="AB18" s="36"/>
-      <c r="AC18" s="36"/>
-      <c r="AD18" s="36"/>
-      <c r="AE18" s="36"/>
-      <c r="AF18" s="36"/>
-      <c r="AG18" s="36"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="35"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="35"/>
+      <c r="Z18" s="35"/>
+      <c r="AA18" s="35"/>
+      <c r="AB18" s="35"/>
+      <c r="AC18" s="35"/>
+      <c r="AD18" s="35"/>
+      <c r="AE18" s="35"/>
+      <c r="AF18" s="35"/>
+      <c r="AG18" s="35"/>
     </row>
     <row r="19" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
-      <c r="Q19" s="47"/>
-      <c r="R19" s="47"/>
-      <c r="S19" s="46"/>
-      <c r="T19" s="46"/>
-      <c r="U19" s="46"/>
-      <c r="V19" s="48" t="s">
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="35"/>
+      <c r="N19" s="35"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="W19" s="46" t="s">
+      <c r="W19" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="X19" s="48" t="s">
+      <c r="X19" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="36"/>
-      <c r="AA19" s="36"/>
-      <c r="AB19" s="36"/>
-      <c r="AC19" s="36"/>
-      <c r="AD19" s="36"/>
-      <c r="AE19" s="36"/>
-      <c r="AF19" s="36"/>
-      <c r="AG19" s="36"/>
+      <c r="Y19" s="35"/>
+      <c r="Z19" s="35"/>
+      <c r="AA19" s="35"/>
+      <c r="AB19" s="35"/>
+      <c r="AC19" s="35"/>
+      <c r="AD19" s="35"/>
+      <c r="AE19" s="35"/>
+      <c r="AF19" s="35"/>
+      <c r="AG19" s="35"/>
     </row>
     <row r="20" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A20" s="17"/>
       <c r="B20" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
-      <c r="Y20" s="49"/>
-      <c r="Z20" s="49"/>
-      <c r="AA20" s="49"/>
-      <c r="AB20" s="49"/>
-      <c r="AC20" s="49"/>
-      <c r="AD20" s="49"/>
-      <c r="AE20" s="49"/>
-      <c r="AF20" s="36"/>
-      <c r="AG20" s="36"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="35"/>
+      <c r="U20" s="35"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="35"/>
+      <c r="X20" s="35"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="48"/>
+      <c r="AD20" s="48"/>
+      <c r="AE20" s="48"/>
+      <c r="AF20" s="35"/>
+      <c r="AG20" s="35"/>
     </row>
     <row r="21" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>3.1</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
-      <c r="S21" s="36"/>
-      <c r="T21" s="36"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="36"/>
-      <c r="W21" s="36"/>
-      <c r="X21" s="36"/>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="51" t="s">
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="35"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="35"/>
+      <c r="P21" s="35"/>
+      <c r="Q21" s="35"/>
+      <c r="R21" s="35"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="35"/>
+      <c r="U21" s="35"/>
+      <c r="V21" s="35"/>
+      <c r="W21" s="35"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="49"/>
+      <c r="Z21" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="AA21" s="52"/>
-      <c r="AB21" s="36"/>
-      <c r="AC21" s="36"/>
-      <c r="AD21" s="36"/>
-      <c r="AE21" s="36"/>
-      <c r="AF21" s="36"/>
-      <c r="AG21" s="36"/>
+      <c r="AA21" s="51"/>
+      <c r="AB21" s="35"/>
+      <c r="AC21" s="35"/>
+      <c r="AD21" s="35"/>
+      <c r="AE21" s="35"/>
+      <c r="AF21" s="35"/>
+      <c r="AG21" s="35"/>
     </row>
     <row r="22" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
@@ -1994,283 +2027,283 @@
       <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="36"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="50"/>
-      <c r="Z22" s="50"/>
-      <c r="AA22" s="50"/>
-      <c r="AB22" s="50"/>
-      <c r="AC22" s="36"/>
-      <c r="AD22" s="36"/>
-      <c r="AE22" s="53"/>
-      <c r="AF22" s="36"/>
-      <c r="AG22" s="36"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="49"/>
+      <c r="Z22" s="49"/>
+      <c r="AA22" s="49"/>
+      <c r="AB22" s="49"/>
+      <c r="AC22" s="35"/>
+      <c r="AD22" s="35"/>
+      <c r="AE22" s="52"/>
+      <c r="AF22" s="35"/>
+      <c r="AG22" s="35"/>
     </row>
     <row r="23" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>3.3</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
-      <c r="S23" s="36"/>
-      <c r="T23" s="36"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="36"/>
-      <c r="W23" s="36"/>
-      <c r="X23" s="36"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="36"/>
-      <c r="AA23" s="36"/>
-      <c r="AB23" s="50"/>
-      <c r="AC23" s="54" t="s">
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
+      <c r="X23" s="35"/>
+      <c r="Y23" s="35"/>
+      <c r="Z23" s="35"/>
+      <c r="AA23" s="35"/>
+      <c r="AB23" s="49"/>
+      <c r="AC23" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="AD23" s="50" t="s">
+      <c r="AD23" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="AE23" s="54" t="s">
+      <c r="AE23" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="AF23" s="36"/>
-      <c r="AG23" s="36"/>
+      <c r="AF23" s="35"/>
+      <c r="AG23" s="35"/>
     </row>
     <row r="24" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
-      <c r="A24" s="28"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
-      <c r="R24" s="55"/>
-      <c r="S24" s="55"/>
-      <c r="T24" s="55"/>
-      <c r="U24" s="55"/>
-      <c r="V24" s="55"/>
-      <c r="W24" s="55"/>
-      <c r="X24" s="55"/>
-      <c r="Y24" s="55"/>
-      <c r="Z24" s="55"/>
-      <c r="AA24" s="55"/>
-      <c r="AB24" s="55"/>
-      <c r="AC24" s="55"/>
-      <c r="AD24" s="55"/>
-      <c r="AE24" s="55"/>
-      <c r="AF24" s="55"/>
-      <c r="AG24" s="55"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="54"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="54"/>
+      <c r="T24" s="54"/>
+      <c r="U24" s="54"/>
+      <c r="V24" s="54"/>
+      <c r="W24" s="54"/>
+      <c r="X24" s="54"/>
+      <c r="Y24" s="54"/>
+      <c r="Z24" s="54"/>
+      <c r="AA24" s="54"/>
+      <c r="AB24" s="54"/>
+      <c r="AC24" s="54"/>
+      <c r="AD24" s="54"/>
+      <c r="AE24" s="54"/>
+      <c r="AF24" s="54"/>
+      <c r="AG24" s="54"/>
     </row>
     <row r="25" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>3.1</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="61" t="s">
+      <c r="C25" s="35"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="K25" s="56" t="s">
+      <c r="K25" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="L25" s="61" t="s">
+      <c r="L25" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="60"/>
-      <c r="U25" s="60"/>
-      <c r="V25" s="60"/>
-      <c r="W25" s="60"/>
-      <c r="X25" s="60"/>
-      <c r="Y25" s="60"/>
-      <c r="Z25" s="60"/>
-      <c r="AA25" s="60"/>
-      <c r="AB25" s="60"/>
-      <c r="AC25" s="60"/>
-      <c r="AD25" s="60"/>
-      <c r="AE25" s="60"/>
-      <c r="AF25" s="60"/>
-      <c r="AG25" s="60"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="59"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="59"/>
+      <c r="Y25" s="59"/>
+      <c r="Z25" s="59"/>
+      <c r="AA25" s="59"/>
+      <c r="AB25" s="59"/>
+      <c r="AC25" s="59"/>
+      <c r="AD25" s="59"/>
+      <c r="AE25" s="59"/>
+      <c r="AF25" s="59"/>
+      <c r="AG25" s="59"/>
     </row>
     <row r="26" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="57" t="s">
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
-      <c r="P26" s="36"/>
-      <c r="Q26" s="36"/>
-      <c r="R26" s="36"/>
-      <c r="S26" s="36"/>
-      <c r="T26" s="36"/>
-      <c r="U26" s="36"/>
-      <c r="V26" s="36"/>
-      <c r="W26" s="36"/>
-      <c r="X26" s="36"/>
-      <c r="Y26" s="36"/>
-      <c r="Z26" s="42"/>
-      <c r="AA26" s="58"/>
-      <c r="AB26" s="58"/>
-      <c r="AC26" s="58"/>
-      <c r="AD26" s="58"/>
-      <c r="AE26" s="58"/>
-      <c r="AF26" s="58"/>
-      <c r="AG26" s="58"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35"/>
+      <c r="X26" s="35"/>
+      <c r="Y26" s="35"/>
+      <c r="Z26" s="41"/>
+      <c r="AA26" s="57"/>
+      <c r="AB26" s="57"/>
+      <c r="AC26" s="57"/>
+      <c r="AD26" s="57"/>
+      <c r="AE26" s="57"/>
+      <c r="AF26" s="57"/>
+      <c r="AG26" s="57"/>
     </row>
     <row r="27" spans="1:33" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>4.2</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="36"/>
-      <c r="P27" s="36"/>
-      <c r="Q27" s="36"/>
-      <c r="R27" s="36"/>
-      <c r="S27" s="36"/>
-      <c r="T27" s="36"/>
-      <c r="U27" s="36"/>
-      <c r="V27" s="56"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="57" t="s">
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
+      <c r="V27" s="55"/>
+      <c r="W27" s="55"/>
+      <c r="X27" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="Y27" s="36"/>
-      <c r="Z27" s="36"/>
-      <c r="AA27" s="36"/>
-      <c r="AB27" s="36"/>
-      <c r="AC27" s="36"/>
-      <c r="AD27" s="36"/>
-      <c r="AE27" s="36"/>
-      <c r="AF27" s="36"/>
-      <c r="AG27" s="36"/>
+      <c r="Y27" s="35"/>
+      <c r="Z27" s="35"/>
+      <c r="AA27" s="35"/>
+      <c r="AB27" s="35"/>
+      <c r="AC27" s="35"/>
+      <c r="AD27" s="35"/>
+      <c r="AE27" s="35"/>
+      <c r="AF27" s="35"/>
+      <c r="AG27" s="35"/>
     </row>
     <row r="28" spans="1:33" ht="14" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>4.3</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-      <c r="M28" s="36"/>
-      <c r="N28" s="36"/>
-      <c r="O28" s="36"/>
-      <c r="P28" s="36"/>
-      <c r="Q28" s="36"/>
-      <c r="R28" s="36"/>
-      <c r="S28" s="36"/>
-      <c r="T28" s="36"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="36"/>
-      <c r="W28" s="36"/>
-      <c r="X28" s="36"/>
-      <c r="Y28" s="36"/>
-      <c r="Z28" s="36"/>
-      <c r="AA28" s="36"/>
-      <c r="AB28" s="36"/>
-      <c r="AC28" s="36"/>
-      <c r="AD28" s="36"/>
-      <c r="AE28" s="56"/>
-      <c r="AF28" s="57"/>
-      <c r="AG28" s="57" t="s">
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
+      <c r="V28" s="35"/>
+      <c r="W28" s="35"/>
+      <c r="X28" s="35"/>
+      <c r="Y28" s="35"/>
+      <c r="Z28" s="35"/>
+      <c r="AA28" s="35"/>
+      <c r="AB28" s="35"/>
+      <c r="AC28" s="35"/>
+      <c r="AD28" s="35"/>
+      <c r="AE28" s="55"/>
+      <c r="AF28" s="56"/>
+      <c r="AG28" s="56" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.15">
-      <c r="B31" s="59"/>
+      <c r="B31" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2283,7 +2316,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2444,7 +2477,7 @@
         <v>600</v>
       </c>
       <c r="D9" s="20">
-        <f>$B9*$C9</f>
+        <f t="shared" si="0"/>
         <v>18000</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -2456,14 +2489,14 @@
         <v>33</v>
       </c>
       <c r="B10" s="22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="20">
         <v>800</v>
       </c>
       <c r="D10" s="20">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2400</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>50</v>
@@ -2474,14 +2507,14 @@
         <v>34</v>
       </c>
       <c r="B11" s="22">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" s="20">
         <v>800</v>
       </c>
       <c r="D11" s="20">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>2400</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>50</v>
@@ -2515,7 +2548,7 @@
       <c r="C13" s="21"/>
       <c r="D13" s="24">
         <f>SUM(D2:D12)</f>
-        <v>197000</v>
+        <v>193800</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -2529,14 +2562,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="26">
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64">
         <f>SUM(D13:D14)</f>
-        <v>257000</v>
+        <v>253800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>